<commit_message>
테이블 수정 및 DDL작성_20181018 12:42
</commit_message>
<xml_diff>
--- a/database/물류시스템DB.xlsx
+++ b/database/물류시스템DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="72" windowWidth="18312" windowHeight="11676" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="72" windowWidth="18312" windowHeight="11676" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="회사테이블" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="376">
   <si>
     <t>테이블명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1508,6 +1508,33 @@
   </si>
   <si>
     <t>코드타입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">primary key </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">identity(1,1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>auto increment</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2027,7 +2054,7 @@
   <cols>
     <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.19921875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2068,7 +2095,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>375</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
@@ -4304,7 +4331,7 @@
   <cols>
     <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4344,7 +4371,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>375</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
@@ -4615,7 +4642,7 @@
   <cols>
     <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4655,7 +4682,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>375</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>62</v>
@@ -5689,7 +5716,7 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0"/>
+    <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
@@ -5889,18 +5916,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet7"/>
+  <sheetPr codeName="Sheet7">
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
     <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5940,7 +5967,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>375</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>

</xml_diff>